<commit_message>
-enh made some changes to the bom
</commit_message>
<xml_diff>
--- a/BOM Testapparaat.xlsx
+++ b/BOM Testapparaat.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="150">
   <si>
     <t xml:space="preserve">Testapparaat APPS</t>
   </si>
@@ -115,27 +115,6 @@
     <t xml:space="preserve">MOUSER</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color rgb="FF0000FF"/>
-        <rFont val="Verdana"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">MOUSER</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <rFont val="Verdana"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">, DIGIKEY</t>
-    </r>
-  </si>
-  <si>
     <t xml:space="preserve">Ker. Condensator 100n</t>
   </si>
   <si>
@@ -220,18 +199,18 @@
     <t xml:space="preserve">Pinheader voor externe FB modules</t>
   </si>
   <si>
+    <t xml:space="preserve">2,54mm pitch, 2 rijen 24 posities</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pinheader 02x06</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pinheader voor debug probe</t>
+  </si>
+  <si>
     <t xml:space="preserve">2,54mm pitch, 2 rijen 12 posities</t>
   </si>
   <si>
-    <t xml:space="preserve">Pinheader 02x06</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pinheader voor debug probe</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2,54mm pitch, 2 rijen 6 posities</t>
-  </si>
-  <si>
     <t xml:space="preserve">Pinheader 01x04</t>
   </si>
   <si>
@@ -256,7 +235,7 @@
     <t xml:space="preserve">Pinheader voor display shield</t>
   </si>
   <si>
-    <t xml:space="preserve">2,54mm pitch, 2 rijen 13 posities</t>
+    <t xml:space="preserve">2,54mm pitch, 2 rijen 26 posities</t>
   </si>
   <si>
     <t xml:space="preserve">Pinheader 02x08</t>
@@ -265,7 +244,7 @@
     <t xml:space="preserve">Pinheader voor knoppen en rotary encoder</t>
   </si>
   <si>
-    <t xml:space="preserve">2,54mm pitch, 2 rijen 8 posities</t>
+    <t xml:space="preserve">2,54mm pitch, 2 rijen 16 posities</t>
   </si>
   <si>
     <t xml:space="preserve">Pinheader 01x08</t>
@@ -343,7 +322,7 @@
     <t xml:space="preserve">3,3uH SMD</t>
   </si>
   <si>
-    <t xml:space="preserve">LMR50410YFQDBVRQ1</t>
+    <t xml:space="preserve">TPS56428RHLR</t>
   </si>
   <si>
     <t xml:space="preserve">dc/dc regulator ic (adj)</t>
@@ -400,9 +379,6 @@
     <t xml:space="preserve">91k, SMD</t>
   </si>
   <si>
-    <t xml:space="preserve">MOUSER, DIGIKEY</t>
-  </si>
-  <si>
     <t xml:space="preserve">Weerstand 43k</t>
   </si>
   <si>
@@ -421,7 +397,7 @@
     <t xml:space="preserve">Weerstand 1%</t>
   </si>
   <si>
-    <t xml:space="preserve">220, SMD</t>
+    <t xml:space="preserve">220R, SMD</t>
   </si>
   <si>
     <t xml:space="preserve">SPST Drukknop</t>
@@ -482,6 +458,15 @@
   </si>
   <si>
     <t xml:space="preserve">SMD, 2-ch</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Adapter 15V 1,6A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Voedingsadapter voor opladen accu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RS</t>
   </si>
   <si>
     <t xml:space="preserve">Subtotaal:</t>
@@ -500,7 +485,7 @@
     <numFmt numFmtId="166" formatCode="d/m/yyyy"/>
     <numFmt numFmtId="167" formatCode="_ &quot;€ &quot;* #,##0.00_ ;_ &quot;€ &quot;* \-#,##0.00_ ;_ &quot;€ &quot;* \-??_ ;_ @_ "/>
   </numFmts>
-  <fonts count="11">
+  <fonts count="12">
     <font>
       <sz val="10"/>
       <name val="Verdana"/>
@@ -555,6 +540,13 @@
     <font>
       <sz val="8"/>
       <color rgb="FF0000FF"/>
+      <name val="Verdana"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FF000000"/>
       <name val="Verdana"/>
       <family val="2"/>
       <charset val="1"/>
@@ -843,56 +835,56 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="61">
+  <cellXfs count="62">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="3" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="3" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="right" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -928,7 +920,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="right" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -936,75 +928,75 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="3" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="3" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="3" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="3" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="6" fillId="3" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="6" fillId="3" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="6" fillId="3" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="6" fillId="3" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="4" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="4" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="4" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="4" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="4" borderId="13" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="4" borderId="13" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="4" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="4" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="4" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="4" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="7" fillId="4" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="7" fillId="4" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="7" fillId="4" borderId="16" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="7" fillId="4" borderId="16" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1028,7 +1020,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="4" fillId="0" borderId="20" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="167" fontId="4" fillId="0" borderId="20" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1052,39 +1044,43 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="23" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="24" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="9" fillId="0" borderId="25" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="10" fillId="3" borderId="26" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="10" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="7" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="10" fillId="3" borderId="27" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="false" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="23" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="24" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="10" fillId="0" borderId="25" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="11" fillId="3" borderId="26" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="10" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="7" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="11" fillId="3" borderId="27" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1161,14 +1157,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="true"/>
   </sheetPr>
-  <dimension ref="A1:R164"/>
+  <dimension ref="A1:R165"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="R59" activeCellId="0" sqref="R59"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D15" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I38" activeCellId="0" sqref="I38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.50390625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1513,7 +1509,7 @@
       </c>
       <c r="H14" s="43"/>
       <c r="I14" s="44" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="J14" s="12"/>
       <c r="K14" s="43" t="n">
@@ -1533,15 +1529,15 @@
     </row>
     <row r="15" customFormat="false" ht="9.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="47" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B15" s="12"/>
       <c r="C15" s="48" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D15" s="12"/>
       <c r="E15" s="47" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F15" s="12"/>
       <c r="G15" s="49" t="s">
@@ -1549,7 +1545,7 @@
       </c>
       <c r="H15" s="49"/>
       <c r="I15" s="50" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="J15" s="12"/>
       <c r="K15" s="49" t="n">
@@ -1569,15 +1565,15 @@
     </row>
     <row r="16" customFormat="false" ht="9.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="47" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B16" s="12"/>
       <c r="C16" s="48" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D16" s="12"/>
       <c r="E16" s="47" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F16" s="12"/>
       <c r="G16" s="49" t="s">
@@ -1585,7 +1581,7 @@
       </c>
       <c r="H16" s="49"/>
       <c r="I16" s="50" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="J16" s="12"/>
       <c r="K16" s="49" t="n">
@@ -1605,15 +1601,15 @@
     </row>
     <row r="17" customFormat="false" ht="9.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="47" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B17" s="12"/>
       <c r="C17" s="48" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D17" s="12"/>
       <c r="E17" s="47" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F17" s="12"/>
       <c r="G17" s="49" t="s">
@@ -1621,7 +1617,7 @@
       </c>
       <c r="H17" s="49"/>
       <c r="I17" s="50" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="J17" s="12"/>
       <c r="K17" s="49" t="n">
@@ -1641,15 +1637,15 @@
     </row>
     <row r="18" customFormat="false" ht="9.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="47" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B18" s="12"/>
       <c r="C18" s="48" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D18" s="12"/>
       <c r="E18" s="47" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F18" s="12"/>
       <c r="G18" s="49" t="s">
@@ -1657,7 +1653,7 @@
       </c>
       <c r="H18" s="49"/>
       <c r="I18" s="50" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="J18" s="12"/>
       <c r="K18" s="49" t="n">
@@ -1677,15 +1673,15 @@
     </row>
     <row r="19" customFormat="false" ht="9.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="47" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B19" s="12"/>
       <c r="C19" s="48" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D19" s="12"/>
       <c r="E19" s="47" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F19" s="12"/>
       <c r="G19" s="49" t="s">
@@ -1693,7 +1689,7 @@
       </c>
       <c r="H19" s="49"/>
       <c r="I19" s="50" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="J19" s="12"/>
       <c r="K19" s="49" t="n">
@@ -1713,15 +1709,15 @@
     </row>
     <row r="20" customFormat="false" ht="9.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="47" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B20" s="12"/>
       <c r="C20" s="48" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D20" s="12"/>
       <c r="E20" s="47" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F20" s="12"/>
       <c r="G20" s="49" t="s">
@@ -1729,7 +1725,7 @@
       </c>
       <c r="H20" s="49"/>
       <c r="I20" s="50" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="J20" s="12"/>
       <c r="K20" s="49" t="n">
@@ -1749,15 +1745,15 @@
     </row>
     <row r="21" customFormat="false" ht="9.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="47" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B21" s="12"/>
       <c r="C21" s="48" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D21" s="12"/>
       <c r="E21" s="47" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F21" s="12"/>
       <c r="G21" s="49" t="s">
@@ -1765,7 +1761,7 @@
       </c>
       <c r="H21" s="49"/>
       <c r="I21" s="50" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="J21" s="12"/>
       <c r="K21" s="49" t="n">
@@ -1785,15 +1781,15 @@
     </row>
     <row r="22" customFormat="false" ht="9.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="47" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B22" s="12"/>
       <c r="C22" s="48" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D22" s="12"/>
       <c r="E22" s="47" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F22" s="12"/>
       <c r="G22" s="49"/>
@@ -1815,22 +1811,24 @@
     </row>
     <row r="23" customFormat="false" ht="9.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="47" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B23" s="12"/>
       <c r="C23" s="48" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D23" s="12"/>
       <c r="E23" s="47" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F23" s="12"/>
       <c r="G23" s="49" t="s">
         <v>29</v>
       </c>
       <c r="H23" s="49"/>
-      <c r="I23" s="49"/>
+      <c r="I23" s="50" t="s">
+        <v>29</v>
+      </c>
       <c r="J23" s="12"/>
       <c r="K23" s="49" t="n">
         <v>1</v>
@@ -1838,24 +1836,26 @@
       <c r="L23" s="12"/>
       <c r="M23" s="49"/>
       <c r="N23" s="12"/>
-      <c r="O23" s="45"/>
+      <c r="O23" s="45" t="n">
+        <v>0.21</v>
+      </c>
       <c r="P23" s="25"/>
       <c r="Q23" s="46" t="n">
         <f aca="false">K23*O23</f>
-        <v>0</v>
+        <v>0.21</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="9.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="47" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B24" s="12"/>
       <c r="C24" s="48" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D24" s="12"/>
       <c r="E24" s="47" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F24" s="12"/>
       <c r="G24" s="49" t="s">
@@ -1863,7 +1863,7 @@
       </c>
       <c r="H24" s="49"/>
       <c r="I24" s="50" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="J24" s="12"/>
       <c r="K24" s="49" t="n">
@@ -1883,15 +1883,15 @@
     </row>
     <row r="25" customFormat="false" ht="9.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="47" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B25" s="12"/>
       <c r="C25" s="48" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D25" s="12"/>
       <c r="E25" s="47" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F25" s="12"/>
       <c r="G25" s="49" t="s">
@@ -1899,7 +1899,7 @@
       </c>
       <c r="H25" s="49"/>
       <c r="I25" s="50" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="J25" s="12"/>
       <c r="K25" s="49" t="n">
@@ -1919,22 +1919,24 @@
     </row>
     <row r="26" customFormat="false" ht="12.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A26" s="47" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B26" s="12"/>
       <c r="C26" s="48" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D26" s="12"/>
       <c r="E26" s="47" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F26" s="12"/>
       <c r="G26" s="49" t="s">
         <v>29</v>
       </c>
       <c r="H26" s="49"/>
-      <c r="I26" s="49"/>
+      <c r="I26" s="50" t="s">
+        <v>29</v>
+      </c>
       <c r="J26" s="12"/>
       <c r="K26" s="49" t="n">
         <v>2</v>
@@ -1942,31 +1944,35 @@
       <c r="L26" s="12"/>
       <c r="M26" s="49"/>
       <c r="N26" s="12"/>
-      <c r="O26" s="45"/>
+      <c r="O26" s="45" t="n">
+        <v>0.14</v>
+      </c>
       <c r="P26" s="25"/>
       <c r="Q26" s="46" t="n">
         <f aca="false">K26*O26</f>
-        <v>0</v>
+        <v>0.28</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A27" s="47" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B27" s="12"/>
       <c r="C27" s="48" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D27" s="12"/>
       <c r="E27" s="47" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F27" s="12"/>
       <c r="G27" s="49" t="s">
         <v>29</v>
       </c>
       <c r="H27" s="49"/>
-      <c r="I27" s="49"/>
+      <c r="I27" s="50" t="s">
+        <v>29</v>
+      </c>
       <c r="J27" s="12"/>
       <c r="K27" s="49" t="n">
         <v>1</v>
@@ -1974,31 +1980,35 @@
       <c r="L27" s="12"/>
       <c r="M27" s="49"/>
       <c r="N27" s="12"/>
-      <c r="O27" s="45"/>
+      <c r="O27" s="45" t="n">
+        <v>0.17</v>
+      </c>
       <c r="P27" s="25"/>
       <c r="Q27" s="46" t="n">
         <f aca="false">K27*O27</f>
-        <v>0</v>
+        <v>0.17</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A28" s="47" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B28" s="12"/>
       <c r="C28" s="48" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D28" s="12"/>
       <c r="E28" s="47" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F28" s="12"/>
       <c r="G28" s="49" t="s">
         <v>29</v>
       </c>
       <c r="H28" s="49"/>
-      <c r="I28" s="49"/>
+      <c r="I28" s="50" t="s">
+        <v>29</v>
+      </c>
       <c r="J28" s="12"/>
       <c r="K28" s="49" t="n">
         <v>1</v>
@@ -2006,31 +2016,35 @@
       <c r="L28" s="12"/>
       <c r="M28" s="49"/>
       <c r="N28" s="12"/>
-      <c r="O28" s="45"/>
+      <c r="O28" s="45" t="n">
+        <v>1.38</v>
+      </c>
       <c r="P28" s="25"/>
       <c r="Q28" s="46" t="n">
         <f aca="false">K28*O28</f>
-        <v>0</v>
+        <v>1.38</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A29" s="47" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B29" s="12"/>
       <c r="C29" s="48" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D29" s="12"/>
       <c r="E29" s="47" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F29" s="12"/>
       <c r="G29" s="49" t="s">
         <v>29</v>
       </c>
       <c r="H29" s="49"/>
-      <c r="I29" s="49"/>
+      <c r="I29" s="50" t="s">
+        <v>29</v>
+      </c>
       <c r="J29" s="12"/>
       <c r="K29" s="49" t="n">
         <v>1</v>
@@ -2038,31 +2052,35 @@
       <c r="L29" s="12"/>
       <c r="M29" s="49"/>
       <c r="N29" s="12"/>
-      <c r="O29" s="45"/>
+      <c r="O29" s="45" t="n">
+        <v>0.52</v>
+      </c>
       <c r="P29" s="25"/>
       <c r="Q29" s="46" t="n">
         <f aca="false">K29*O29</f>
-        <v>0</v>
+        <v>0.52</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A30" s="47" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B30" s="12"/>
       <c r="C30" s="48" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D30" s="12"/>
       <c r="E30" s="47" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F30" s="12"/>
       <c r="G30" s="49" t="s">
         <v>29</v>
       </c>
       <c r="H30" s="49"/>
-      <c r="I30" s="49"/>
+      <c r="I30" s="50" t="s">
+        <v>29</v>
+      </c>
       <c r="J30" s="12"/>
       <c r="K30" s="49" t="n">
         <v>1</v>
@@ -2070,28 +2088,30 @@
       <c r="L30" s="12"/>
       <c r="M30" s="49"/>
       <c r="N30" s="12"/>
-      <c r="O30" s="45"/>
+      <c r="O30" s="45" t="n">
+        <v>0.27</v>
+      </c>
       <c r="P30" s="25"/>
       <c r="Q30" s="46" t="n">
         <f aca="false">K30*O30</f>
-        <v>0</v>
+        <v>0.27</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A31" s="47" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B31" s="12"/>
       <c r="C31" s="48" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D31" s="12"/>
       <c r="E31" s="47" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F31" s="12"/>
       <c r="G31" s="49" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="H31" s="49"/>
       <c r="I31" s="49"/>
@@ -2111,15 +2131,15 @@
     </row>
     <row r="32" customFormat="false" ht="9.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A32" s="47" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B32" s="12"/>
       <c r="C32" s="48" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D32" s="12"/>
       <c r="E32" s="47" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F32" s="12"/>
       <c r="G32" s="49" t="s">
@@ -2127,7 +2147,7 @@
       </c>
       <c r="H32" s="49"/>
       <c r="I32" s="50" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="J32" s="12"/>
       <c r="K32" s="49" t="n">
@@ -2147,15 +2167,15 @@
     </row>
     <row r="33" customFormat="false" ht="9.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A33" s="47" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B33" s="12"/>
       <c r="C33" s="48" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D33" s="12"/>
       <c r="E33" s="47" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="F33" s="12"/>
       <c r="G33" s="49" t="s">
@@ -2163,7 +2183,7 @@
       </c>
       <c r="H33" s="49"/>
       <c r="I33" s="50" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="J33" s="12"/>
       <c r="K33" s="49" t="n">
@@ -2183,15 +2203,15 @@
     </row>
     <row r="34" customFormat="false" ht="9.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A34" s="47" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B34" s="12"/>
       <c r="C34" s="48" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D34" s="12"/>
       <c r="E34" s="47" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F34" s="12"/>
       <c r="G34" s="49" t="s">
@@ -2199,7 +2219,7 @@
       </c>
       <c r="H34" s="49"/>
       <c r="I34" s="50" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="J34" s="12"/>
       <c r="K34" s="49" t="n">
@@ -2219,15 +2239,15 @@
     </row>
     <row r="35" customFormat="false" ht="9.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A35" s="47" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B35" s="12"/>
       <c r="C35" s="48" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D35" s="12"/>
       <c r="E35" s="47" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F35" s="12"/>
       <c r="G35" s="49" t="s">
@@ -2251,15 +2271,15 @@
     </row>
     <row r="36" customFormat="false" ht="9.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A36" s="47" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B36" s="12"/>
       <c r="C36" s="48" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D36" s="12"/>
       <c r="E36" s="47" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F36" s="12"/>
       <c r="G36" s="49" t="s">
@@ -2283,15 +2303,15 @@
     </row>
     <row r="37" customFormat="false" ht="9.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A37" s="47" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B37" s="12"/>
       <c r="C37" s="48" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D37" s="12"/>
       <c r="E37" s="47" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F37" s="12"/>
       <c r="G37" s="49" t="s">
@@ -2315,22 +2335,24 @@
     </row>
     <row r="38" customFormat="false" ht="9.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A38" s="47" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B38" s="12"/>
       <c r="C38" s="48" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D38" s="12"/>
       <c r="E38" s="47" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="F38" s="12"/>
       <c r="G38" s="49" t="s">
         <v>29</v>
       </c>
       <c r="H38" s="49"/>
-      <c r="I38" s="49"/>
+      <c r="I38" s="50" t="s">
+        <v>29</v>
+      </c>
       <c r="J38" s="12"/>
       <c r="K38" s="49" t="n">
         <v>2</v>
@@ -2338,31 +2360,35 @@
       <c r="L38" s="12"/>
       <c r="M38" s="49"/>
       <c r="N38" s="12"/>
-      <c r="O38" s="45"/>
+      <c r="O38" s="45" t="n">
+        <v>1.63</v>
+      </c>
       <c r="P38" s="25"/>
       <c r="Q38" s="46" t="n">
         <f aca="false">K38*O38</f>
-        <v>0</v>
+        <v>3.26</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="9.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A39" s="47" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B39" s="12"/>
       <c r="C39" s="48" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D39" s="12"/>
       <c r="E39" s="47" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F39" s="12"/>
       <c r="G39" s="49" t="s">
         <v>29</v>
       </c>
       <c r="H39" s="49"/>
-      <c r="I39" s="49"/>
+      <c r="I39" s="50" t="s">
+        <v>29</v>
+      </c>
       <c r="J39" s="12"/>
       <c r="K39" s="49" t="n">
         <v>3</v>
@@ -2370,31 +2396,35 @@
       <c r="L39" s="12"/>
       <c r="M39" s="49"/>
       <c r="N39" s="12"/>
-      <c r="O39" s="45"/>
+      <c r="O39" s="45" t="n">
+        <v>0.17</v>
+      </c>
       <c r="P39" s="25"/>
       <c r="Q39" s="46" t="n">
         <f aca="false">K39*O39</f>
-        <v>0</v>
+        <v>0.51</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="9.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A40" s="47" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B40" s="12"/>
       <c r="C40" s="48" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D40" s="12"/>
       <c r="E40" s="47" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F40" s="12"/>
       <c r="G40" s="49" t="s">
         <v>29</v>
       </c>
       <c r="H40" s="49"/>
-      <c r="I40" s="49"/>
+      <c r="I40" s="50" t="s">
+        <v>29</v>
+      </c>
       <c r="J40" s="12"/>
       <c r="K40" s="49" t="n">
         <v>3</v>
@@ -2402,31 +2432,35 @@
       <c r="L40" s="12"/>
       <c r="M40" s="49"/>
       <c r="N40" s="12"/>
-      <c r="O40" s="45"/>
+      <c r="O40" s="45" t="n">
+        <v>1.04</v>
+      </c>
       <c r="P40" s="25"/>
       <c r="Q40" s="46" t="n">
         <f aca="false">K40*O40</f>
-        <v>0</v>
+        <v>3.12</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="9.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A41" s="47" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B41" s="12"/>
       <c r="C41" s="48" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D41" s="12"/>
       <c r="E41" s="47" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="F41" s="12"/>
       <c r="G41" s="49" t="s">
         <v>29</v>
       </c>
       <c r="H41" s="49"/>
-      <c r="I41" s="49"/>
+      <c r="I41" s="50" t="s">
+        <v>29</v>
+      </c>
       <c r="J41" s="12"/>
       <c r="K41" s="49" t="n">
         <v>3</v>
@@ -2434,31 +2468,35 @@
       <c r="L41" s="12"/>
       <c r="M41" s="49"/>
       <c r="N41" s="12"/>
-      <c r="O41" s="45"/>
+      <c r="O41" s="45" t="n">
+        <v>0.1</v>
+      </c>
       <c r="P41" s="25"/>
       <c r="Q41" s="46" t="n">
         <f aca="false">K41*O41</f>
-        <v>0</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="9.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A42" s="47" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B42" s="12"/>
       <c r="C42" s="48" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D42" s="12"/>
       <c r="E42" s="47" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="F42" s="12"/>
       <c r="G42" s="49" t="s">
         <v>29</v>
       </c>
       <c r="H42" s="49"/>
-      <c r="I42" s="49"/>
+      <c r="I42" s="50" t="s">
+        <v>29</v>
+      </c>
       <c r="J42" s="12"/>
       <c r="K42" s="49" t="n">
         <v>18</v>
@@ -2466,24 +2504,26 @@
       <c r="L42" s="12"/>
       <c r="M42" s="49"/>
       <c r="N42" s="12"/>
-      <c r="O42" s="45"/>
+      <c r="O42" s="45" t="n">
+        <v>0.1</v>
+      </c>
       <c r="P42" s="25"/>
       <c r="Q42" s="46" t="n">
         <f aca="false">K42*O42</f>
-        <v>0</v>
+        <v>1.8</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="9.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A43" s="47" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B43" s="12"/>
       <c r="C43" s="48" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D43" s="12"/>
       <c r="E43" s="47" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="F43" s="12"/>
       <c r="G43" s="49" t="s">
@@ -2491,7 +2531,7 @@
       </c>
       <c r="H43" s="49"/>
       <c r="I43" s="50" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="J43" s="12"/>
       <c r="K43" s="49" t="n">
@@ -2511,15 +2551,15 @@
     </row>
     <row r="44" customFormat="false" ht="9.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A44" s="47" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B44" s="12"/>
       <c r="C44" s="48" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D44" s="12"/>
       <c r="E44" s="47" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="F44" s="12"/>
       <c r="G44" s="49" t="s">
@@ -2527,7 +2567,7 @@
       </c>
       <c r="H44" s="49"/>
       <c r="I44" s="50" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="J44" s="12"/>
       <c r="K44" s="49" t="n">
@@ -2547,23 +2587,23 @@
     </row>
     <row r="45" customFormat="false" ht="9.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A45" s="47" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B45" s="12"/>
       <c r="C45" s="48" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D45" s="12"/>
       <c r="E45" s="47" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="F45" s="12"/>
       <c r="G45" s="49" t="s">
         <v>29</v>
       </c>
       <c r="H45" s="49"/>
-      <c r="I45" s="49" t="s">
-        <v>119</v>
+      <c r="I45" s="50" t="s">
+        <v>29</v>
       </c>
       <c r="J45" s="12"/>
       <c r="K45" s="49" t="n">
@@ -2572,32 +2612,34 @@
       <c r="L45" s="12"/>
       <c r="M45" s="49"/>
       <c r="N45" s="12"/>
-      <c r="O45" s="45"/>
+      <c r="O45" s="45" t="n">
+        <v>0.1</v>
+      </c>
       <c r="P45" s="25"/>
       <c r="Q45" s="46" t="n">
         <f aca="false">K45*O45</f>
-        <v>0</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="9.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A46" s="47" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B46" s="12"/>
       <c r="C46" s="48" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D46" s="12"/>
       <c r="E46" s="47" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="F46" s="12"/>
       <c r="G46" s="49" t="s">
         <v>29</v>
       </c>
       <c r="H46" s="49"/>
-      <c r="I46" s="49" t="s">
-        <v>119</v>
+      <c r="I46" s="50" t="s">
+        <v>29</v>
       </c>
       <c r="J46" s="12"/>
       <c r="K46" s="49" t="n">
@@ -2606,32 +2648,34 @@
       <c r="L46" s="12"/>
       <c r="M46" s="49"/>
       <c r="N46" s="12"/>
-      <c r="O46" s="45"/>
+      <c r="O46" s="45" t="n">
+        <v>0.1</v>
+      </c>
       <c r="P46" s="25"/>
       <c r="Q46" s="46" t="n">
         <f aca="false">K46*O46</f>
-        <v>0</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="9.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A47" s="47" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B47" s="12"/>
       <c r="C47" s="48" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D47" s="12"/>
       <c r="E47" s="47" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="F47" s="12"/>
       <c r="G47" s="49" t="s">
         <v>29</v>
       </c>
       <c r="H47" s="49"/>
-      <c r="I47" s="49" t="s">
-        <v>119</v>
+      <c r="I47" s="50" t="s">
+        <v>29</v>
       </c>
       <c r="J47" s="12"/>
       <c r="K47" s="49" t="n">
@@ -2640,32 +2684,34 @@
       <c r="L47" s="12"/>
       <c r="M47" s="49"/>
       <c r="N47" s="12"/>
-      <c r="O47" s="45"/>
+      <c r="O47" s="45" t="n">
+        <v>0.1</v>
+      </c>
       <c r="P47" s="25"/>
       <c r="Q47" s="46" t="n">
         <f aca="false">K47*O47</f>
-        <v>0</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="9.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A48" s="47" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B48" s="12"/>
       <c r="C48" s="48" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="D48" s="12"/>
       <c r="E48" s="47" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="F48" s="12"/>
       <c r="G48" s="49" t="s">
         <v>29</v>
       </c>
       <c r="H48" s="49"/>
-      <c r="I48" s="49" t="s">
-        <v>119</v>
+      <c r="I48" s="50" t="s">
+        <v>29</v>
       </c>
       <c r="J48" s="12"/>
       <c r="K48" s="49" t="n">
@@ -2674,24 +2720,26 @@
       <c r="L48" s="12"/>
       <c r="M48" s="49"/>
       <c r="N48" s="12"/>
-      <c r="O48" s="45"/>
+      <c r="O48" s="45" t="n">
+        <v>0.1</v>
+      </c>
       <c r="P48" s="25"/>
       <c r="Q48" s="46" t="n">
         <f aca="false">K48*O48</f>
-        <v>0</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="9.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A49" s="47" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B49" s="12"/>
       <c r="C49" s="48" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="D49" s="12"/>
       <c r="E49" s="47" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="F49" s="12"/>
       <c r="G49" s="49" t="s">
@@ -2699,7 +2747,7 @@
       </c>
       <c r="H49" s="49"/>
       <c r="I49" s="49" t="s">
-        <v>119</v>
+        <v>29</v>
       </c>
       <c r="J49" s="12"/>
       <c r="K49" s="49" t="n">
@@ -2717,15 +2765,15 @@
     </row>
     <row r="50" customFormat="false" ht="9.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A50" s="47" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B50" s="12"/>
       <c r="C50" s="48" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="D50" s="12"/>
       <c r="E50" s="47" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="F50" s="12"/>
       <c r="G50" s="49" t="s">
@@ -2749,22 +2797,24 @@
     </row>
     <row r="51" customFormat="false" ht="9.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A51" s="47" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B51" s="12"/>
       <c r="C51" s="48" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="D51" s="12"/>
       <c r="E51" s="47" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="F51" s="12"/>
       <c r="G51" s="49" t="s">
         <v>29</v>
       </c>
       <c r="H51" s="49"/>
-      <c r="I51" s="49"/>
+      <c r="I51" s="50" t="s">
+        <v>29</v>
+      </c>
       <c r="J51" s="12"/>
       <c r="K51" s="49" t="n">
         <v>2</v>
@@ -2781,22 +2831,24 @@
     </row>
     <row r="52" customFormat="false" ht="9.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A52" s="47" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B52" s="12"/>
       <c r="C52" s="48" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="D52" s="12"/>
       <c r="E52" s="47" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="F52" s="12"/>
       <c r="G52" s="49" t="s">
         <v>29</v>
       </c>
       <c r="H52" s="49"/>
-      <c r="I52" s="49"/>
+      <c r="I52" s="50" t="s">
+        <v>29</v>
+      </c>
       <c r="J52" s="12"/>
       <c r="K52" s="49" t="n">
         <v>1</v>
@@ -2813,22 +2865,24 @@
     </row>
     <row r="53" customFormat="false" ht="9.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A53" s="47" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="B53" s="12"/>
       <c r="C53" s="48" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="D53" s="12"/>
       <c r="E53" s="47" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="F53" s="12"/>
       <c r="G53" s="49" t="s">
         <v>29</v>
       </c>
       <c r="H53" s="49"/>
-      <c r="I53" s="49"/>
+      <c r="I53" s="50" t="s">
+        <v>29</v>
+      </c>
       <c r="J53" s="12"/>
       <c r="K53" s="49" t="n">
         <v>2</v>
@@ -2836,31 +2890,35 @@
       <c r="L53" s="12"/>
       <c r="M53" s="49"/>
       <c r="N53" s="12"/>
-      <c r="O53" s="45"/>
+      <c r="O53" s="45" t="n">
+        <v>1.44</v>
+      </c>
       <c r="P53" s="25"/>
       <c r="Q53" s="46" t="n">
         <f aca="false">K53*O53</f>
-        <v>0</v>
+        <v>2.88</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="9.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A54" s="47" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B54" s="12"/>
       <c r="C54" s="48" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="D54" s="12"/>
       <c r="E54" s="47" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="F54" s="12"/>
       <c r="G54" s="49" t="s">
         <v>29</v>
       </c>
       <c r="H54" s="49"/>
-      <c r="I54" s="49"/>
+      <c r="I54" s="50" t="s">
+        <v>29</v>
+      </c>
       <c r="J54" s="12"/>
       <c r="K54" s="49" t="n">
         <v>3</v>
@@ -2877,15 +2935,15 @@
     </row>
     <row r="55" customFormat="false" ht="9.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A55" s="47" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="B55" s="12"/>
       <c r="C55" s="48" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="D55" s="12"/>
       <c r="E55" s="47" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="F55" s="12"/>
       <c r="G55" s="49" t="s">
@@ -2893,7 +2951,7 @@
       </c>
       <c r="H55" s="49"/>
       <c r="I55" s="50" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="J55" s="12"/>
       <c r="K55" s="49" t="n">
@@ -2911,54 +2969,85 @@
         <v>1.05</v>
       </c>
     </row>
-    <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B56" s="52"/>
-      <c r="C56" s="53"/>
-      <c r="E56" s="53"/>
-      <c r="F56" s="52"/>
-      <c r="J56" s="52"/>
-      <c r="K56" s="53"/>
-      <c r="L56" s="52"/>
-      <c r="M56" s="53"/>
-      <c r="O56" s="54" t="s">
+    <row r="56" customFormat="false" ht="9.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A56" s="47" t="s">
+        <v>145</v>
+      </c>
+      <c r="B56" s="12"/>
+      <c r="C56" s="48" t="s">
+        <v>146</v>
+      </c>
+      <c r="D56" s="12"/>
+      <c r="E56" s="47"/>
+      <c r="F56" s="12"/>
+      <c r="G56" s="49" t="s">
         <v>147</v>
       </c>
-      <c r="P56" s="55"/>
-      <c r="Q56" s="56" t="n">
-        <f aca="false">SUM(Q14:Q55)</f>
-        <v>13.58</v>
+      <c r="H56" s="49"/>
+      <c r="I56" s="52" t="s">
+        <v>147</v>
+      </c>
+      <c r="J56" s="12"/>
+      <c r="K56" s="49" t="n">
+        <v>1</v>
+      </c>
+      <c r="L56" s="12"/>
+      <c r="M56" s="49"/>
+      <c r="N56" s="12"/>
+      <c r="O56" s="51" t="n">
+        <v>15.75</v>
+      </c>
+      <c r="P56" s="25"/>
+      <c r="Q56" s="51" t="n">
+        <f aca="false">K56*O56</f>
+        <v>15.75</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Q57" s="57"/>
+      <c r="B57" s="53"/>
+      <c r="C57" s="54"/>
+      <c r="E57" s="54"/>
+      <c r="F57" s="53"/>
+      <c r="J57" s="53"/>
+      <c r="K57" s="54"/>
+      <c r="L57" s="53"/>
+      <c r="M57" s="54"/>
+      <c r="O57" s="55" t="s">
+        <v>148</v>
+      </c>
+      <c r="P57" s="56"/>
+      <c r="Q57" s="57" t="n">
+        <f aca="false">SUM(Q14:Q56)</f>
+        <v>44.63</v>
+      </c>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A58" s="13"/>
-      <c r="B58" s="58"/>
-      <c r="C58" s="13"/>
-      <c r="D58" s="58"/>
-      <c r="E58" s="13"/>
-      <c r="F58" s="58"/>
-      <c r="G58" s="13"/>
-      <c r="H58" s="13"/>
-      <c r="I58" s="13"/>
-      <c r="J58" s="58"/>
-      <c r="K58" s="13"/>
-      <c r="L58" s="58"/>
-      <c r="M58" s="13"/>
-      <c r="N58" s="58"/>
-      <c r="O58" s="59" t="s">
-        <v>148</v>
-      </c>
-      <c r="P58" s="58"/>
-      <c r="Q58" s="60" t="n">
-        <f aca="false">Q56</f>
-        <v>13.58</v>
-      </c>
-      <c r="R58" s="2"/>
+      <c r="Q58" s="58"/>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Q59" s="1"/>
+      <c r="A59" s="13"/>
+      <c r="B59" s="59"/>
+      <c r="C59" s="13"/>
+      <c r="D59" s="59"/>
+      <c r="E59" s="13"/>
+      <c r="F59" s="59"/>
+      <c r="G59" s="13"/>
+      <c r="H59" s="13"/>
+      <c r="I59" s="13"/>
+      <c r="J59" s="59"/>
+      <c r="K59" s="13"/>
+      <c r="L59" s="59"/>
+      <c r="M59" s="13"/>
+      <c r="N59" s="59"/>
+      <c r="O59" s="60" t="s">
+        <v>149</v>
+      </c>
+      <c r="P59" s="59"/>
+      <c r="Q59" s="61" t="n">
+        <f aca="false">Q57</f>
+        <v>44.63</v>
+      </c>
+      <c r="R59" s="2"/>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="Q60" s="1"/>
@@ -3274,6 +3363,9 @@
     </row>
     <row r="164" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="Q164" s="1"/>
+    </row>
+    <row r="165" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="Q165" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -3291,14 +3383,34 @@
     <hyperlink ref="I19" r:id="rId6" display="MOUSER"/>
     <hyperlink ref="I20" r:id="rId7" display="MOUSER"/>
     <hyperlink ref="I21" r:id="rId8" display="MOUSER"/>
-    <hyperlink ref="I24" r:id="rId9" display="MOUSER"/>
-    <hyperlink ref="I25" r:id="rId10" display="MOUSER"/>
-    <hyperlink ref="I32" r:id="rId11" display="MOUSER"/>
-    <hyperlink ref="I33" r:id="rId12" display="MOUSER"/>
-    <hyperlink ref="I34" r:id="rId13" display="MOUSER"/>
-    <hyperlink ref="I43" r:id="rId14" display="MOUSER"/>
-    <hyperlink ref="I44" r:id="rId15" display="MOUSER"/>
-    <hyperlink ref="I55" r:id="rId16" display="MOUSER"/>
+    <hyperlink ref="I23" r:id="rId9" display="MOUSER"/>
+    <hyperlink ref="I24" r:id="rId10" display="MOUSER"/>
+    <hyperlink ref="I25" r:id="rId11" display="MOUSER"/>
+    <hyperlink ref="I26" r:id="rId12" display="MOUSER"/>
+    <hyperlink ref="I27" r:id="rId13" display="MOUSER"/>
+    <hyperlink ref="I28" r:id="rId14" display="MOUSER"/>
+    <hyperlink ref="I29" r:id="rId15" display="MOUSER"/>
+    <hyperlink ref="I30" r:id="rId16" display="MOUSER"/>
+    <hyperlink ref="I32" r:id="rId17" display="MOUSER"/>
+    <hyperlink ref="I33" r:id="rId18" display="MOUSER"/>
+    <hyperlink ref="I34" r:id="rId19" display="MOUSER"/>
+    <hyperlink ref="I38" r:id="rId20" display="MOUSER"/>
+    <hyperlink ref="I39" r:id="rId21" display="MOUSER"/>
+    <hyperlink ref="I40" r:id="rId22" display="MOUSER"/>
+    <hyperlink ref="I41" r:id="rId23" display="MOUSER"/>
+    <hyperlink ref="I42" r:id="rId24" display="MOUSER"/>
+    <hyperlink ref="I43" r:id="rId25" display="MOUSER"/>
+    <hyperlink ref="I44" r:id="rId26" display="MOUSER"/>
+    <hyperlink ref="I45" r:id="rId27" display="MOUSER"/>
+    <hyperlink ref="I46" r:id="rId28" display="MOUSER"/>
+    <hyperlink ref="I47" r:id="rId29" display="MOUSER"/>
+    <hyperlink ref="I48" r:id="rId30" display="MOUSER"/>
+    <hyperlink ref="I51" r:id="rId31" display="MOUSER"/>
+    <hyperlink ref="I52" r:id="rId32" display="MOUSER"/>
+    <hyperlink ref="I53" r:id="rId33" display="MOUSER"/>
+    <hyperlink ref="I54" r:id="rId34" display="MOUSER"/>
+    <hyperlink ref="I55" r:id="rId35" display="MOUSER"/>
+    <hyperlink ref="I56" r:id="rId36" display="RS"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.25" right="0.25" top="0.25" bottom="0.25" header="0.511811023622047" footer="0.511811023622047"/>

</xml_diff>